<commit_message>
monitoring implementation plan added to memory bank. file structure added. time to get to it
</commit_message>
<xml_diff>
--- a/volatility_comparison/volatility_comparison_formatted.xlsx
+++ b/volatility_comparison/volatility_comparison_formatted.xlsx
@@ -687,34 +687,34 @@
         </is>
       </c>
       <c r="B5" s="3" t="n">
-        <v>331.61719</v>
+        <v>331.89844</v>
       </c>
       <c r="C5" s="3" t="n">
-        <v>110.53906</v>
+        <v>110.63281</v>
       </c>
       <c r="D5" s="3" t="n">
-        <v>110.53906</v>
+        <v>110.63281</v>
       </c>
       <c r="E5" s="3" t="n">
-        <v>110.53906</v>
+        <v>110.63281</v>
       </c>
       <c r="F5" s="3" t="n">
-        <v>110.5390625</v>
+        <v>110.6171875</v>
       </c>
       <c r="G5" s="3" t="n">
-        <v>110.5390625</v>
+        <v>110.6171875</v>
       </c>
       <c r="H5" s="3" t="n">
-        <v>110.5390625</v>
+        <v>110.6171875</v>
       </c>
       <c r="I5" s="3" t="n">
-        <v>110.5390625</v>
+        <v>110.6171875</v>
       </c>
       <c r="J5" s="3" t="n">
-        <v>110.5390625</v>
+        <v>110.6171875</v>
       </c>
       <c r="K5" s="3" t="n">
-        <v>110.5390625</v>
+        <v>110.6171875</v>
       </c>
     </row>
     <row r="6">
@@ -724,34 +724,34 @@
         </is>
       </c>
       <c r="B6" s="3" t="n">
-        <v>6.672069999999986</v>
+        <v>8.406249999999993</v>
       </c>
       <c r="C6" s="3" t="n">
-        <v>0.3482299999999825</v>
+        <v>0.1354199999999865</v>
       </c>
       <c r="D6" s="3" t="n">
-        <v>1.768999999999981</v>
+        <v>3.135419999999994</v>
       </c>
       <c r="E6" s="3" t="n">
-        <v>4.554839999999987</v>
+        <v>5.135419999999987</v>
       </c>
       <c r="F6" s="3" t="n">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
       <c r="G6" s="3" t="n">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
       <c r="H6" s="3" t="n">
-        <v>1.1</v>
+        <v>1</v>
       </c>
       <c r="I6" s="3" t="n">
-        <v>1.1</v>
+        <v>1</v>
       </c>
       <c r="J6" s="3" t="n">
-        <v>3.1</v>
+        <v>3</v>
       </c>
       <c r="K6" s="3" t="n">
-        <v>3.1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7">
@@ -761,34 +761,34 @@
         </is>
       </c>
       <c r="B7" s="3" t="n">
-        <v>0.0182796438356164</v>
+        <v>0.0230308219178082</v>
       </c>
       <c r="C7" s="3" t="n">
-        <v>0.0009540547945205</v>
+        <v>0.0003710136986301</v>
       </c>
       <c r="D7" s="3" t="n">
-        <v>0.0048465753424657</v>
+        <v>0.008590191780821901</v>
       </c>
       <c r="E7" s="3" t="n">
-        <v>0.0124790136986301</v>
+        <v>0.0140696438356164</v>
       </c>
       <c r="F7" s="3" t="n">
-        <v>0.00119047619047619</v>
+        <v>0.0003968253968253968</v>
       </c>
       <c r="G7" s="3" t="n">
-        <v>0.00119047619047619</v>
+        <v>0.0003968253968253968</v>
       </c>
       <c r="H7" s="3" t="n">
-        <v>0.004365079365079365</v>
+        <v>0.003968253968253968</v>
       </c>
       <c r="I7" s="3" t="n">
-        <v>0.004365079365079365</v>
+        <v>0.003968253968253968</v>
       </c>
       <c r="J7" s="3" t="n">
-        <v>0.0123015873015873</v>
+        <v>0.0119047619047619</v>
       </c>
       <c r="K7" s="3" t="n">
-        <v>0.0123015873015873</v>
+        <v>0.0119047619047619</v>
       </c>
     </row>
     <row r="8">
@@ -802,22 +802,22 @@
       <c r="D8" s="3" t="inlineStr"/>
       <c r="E8" s="3" t="inlineStr"/>
       <c r="F8" s="3" t="n">
-        <v>0.7</v>
+        <v>1.2</v>
       </c>
       <c r="G8" s="3" t="n">
-        <v>5</v>
+        <v>8.5</v>
       </c>
       <c r="H8" s="3" t="n">
-        <v>6.5</v>
+        <v>10</v>
       </c>
       <c r="I8" s="3" t="n">
-        <v>12.5</v>
+        <v>17</v>
       </c>
       <c r="J8" s="3" t="n">
-        <v>13.5</v>
+        <v>17</v>
       </c>
       <c r="K8" s="3" t="n">
-        <v>20.5</v>
+        <v>24.5</v>
       </c>
     </row>
     <row r="9">
@@ -832,32 +832,32 @@
       <c r="E9" s="3" t="inlineStr"/>
       <c r="F9" s="3" t="inlineStr">
         <is>
-          <t>0.70</t>
+          <t>1.20</t>
         </is>
       </c>
       <c r="G9" s="3" t="inlineStr">
         <is>
-          <t>5.00</t>
+          <t>8.50</t>
         </is>
       </c>
       <c r="H9" s="3" t="inlineStr">
         <is>
-          <t>6.50</t>
+          <t>10.00</t>
         </is>
       </c>
       <c r="I9" s="3" t="inlineStr">
         <is>
-          <t>12.50</t>
+          <t>17.00</t>
         </is>
       </c>
       <c r="J9" s="3" t="inlineStr">
         <is>
-          <t>13.50</t>
+          <t>17.00</t>
         </is>
       </c>
       <c r="K9" s="3" t="inlineStr">
         <is>
-          <t>20.50</t>
+          <t>24.50</t>
         </is>
       </c>
     </row>
@@ -875,19 +875,19 @@
         <v>0.4</v>
       </c>
       <c r="G10" s="3" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="H10" s="3" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="I10" s="3" t="n">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="J10" s="3" t="n">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="K10" s="3" t="n">
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11">
@@ -901,22 +901,22 @@
       <c r="D11" s="3" t="inlineStr"/>
       <c r="E11" s="3" t="inlineStr"/>
       <c r="F11" s="3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G11" s="3" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="H11" s="3" t="n">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="I11" s="3" t="n">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="J11" s="3" t="n">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="K11" s="3" t="n">
-        <v>21</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12">
@@ -926,25 +926,25 @@
         </is>
       </c>
       <c r="B12" s="5" t="n">
-        <v>23.82815</v>
+        <v>23.70031</v>
       </c>
       <c r="C12" s="5" t="n">
         <v>8.762119999999999</v>
       </c>
       <c r="D12" s="5" t="n">
-        <v>7.27384</v>
+        <v>7.2166</v>
       </c>
       <c r="E12" s="5" t="n">
-        <v>7.7922</v>
+        <v>7.72159</v>
       </c>
       <c r="F12" s="5" t="n">
-        <v>5.53</v>
+        <v>6.59</v>
       </c>
       <c r="G12" s="5" t="n">
-        <v>4.3</v>
+        <v>6.68</v>
       </c>
       <c r="H12" s="5" t="n">
-        <v>7.07</v>
+        <v>8.59</v>
       </c>
       <c r="I12" s="5" t="n">
         <v>7.05</v>
@@ -953,7 +953,7 @@
         <v>6.47</v>
       </c>
       <c r="K12" s="5" t="n">
-        <v>6.76</v>
+        <v>7.36</v>
       </c>
     </row>
     <row r="13">
@@ -968,32 +968,32 @@
       <c r="E13" s="7" t="inlineStr"/>
       <c r="F13" s="7" t="inlineStr">
         <is>
-          <t>5.25</t>
+          <t>8.12</t>
         </is>
       </c>
       <c r="G13" s="7" t="inlineStr">
         <is>
-          <t>4.10</t>
+          <t>7.00</t>
         </is>
       </c>
       <c r="H13" s="7" t="inlineStr">
         <is>
-          <t>7.15</t>
+          <t>8.60</t>
         </is>
       </c>
       <c r="I13" s="7" t="inlineStr">
         <is>
-          <t>6.64</t>
+          <t>8.02</t>
         </is>
       </c>
       <c r="J13" s="7" t="inlineStr">
         <is>
-          <t>6.89</t>
+          <t>7.53</t>
         </is>
       </c>
       <c r="K13" s="7" t="inlineStr">
         <is>
-          <t>6.79</t>
+          <t>7.37</t>
         </is>
       </c>
     </row>
@@ -1008,22 +1008,22 @@
       <c r="D14" s="3" t="inlineStr"/>
       <c r="E14" s="3" t="inlineStr"/>
       <c r="F14" s="3" t="n">
-        <v>0.2800000000000002</v>
+        <v>-1.529999999999999</v>
       </c>
       <c r="G14" s="3" t="n">
-        <v>0.2000000000000002</v>
+        <v>-0.3200000000000003</v>
       </c>
       <c r="H14" s="3" t="n">
-        <v>-0.08000000000000007</v>
+        <v>-0.009999999999999787</v>
       </c>
       <c r="I14" s="3" t="n">
-        <v>0.4100000000000001</v>
+        <v>-0.9699999999999998</v>
       </c>
       <c r="J14" s="3" t="n">
-        <v>-0.4199999999999999</v>
+        <v>-1.06</v>
       </c>
       <c r="K14" s="3" t="n">
-        <v>-0.03000000000000025</v>
+        <v>-0.009999999999999787</v>
       </c>
     </row>
   </sheetData>

</xml_diff>